<commit_message>
Grafo con informação das conexões e velocidade (Giga)
</commit_message>
<xml_diff>
--- a/planilhas/core01.xlsx
+++ b/planilhas/core01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade\IC-GRAFOS\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4934632C-2C65-48CC-A642-27D4DAB63272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80E47F5-413C-420F-B63C-0B6D7F0602C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PORTAS_CORE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="41">
   <si>
     <t>Porta</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>MGMT_DELL</t>
+  </si>
+  <si>
+    <t>Fonte</t>
+  </si>
+  <si>
+    <t>CORE01</t>
   </si>
 </sst>
 </file>
@@ -502,674 +508,822 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F992"/>
+  <dimension ref="A1:G992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H68" sqref="A50:H68"/>
+      <selection activeCell="A3" sqref="A3:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="1" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="2">
+      <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>43675</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="2">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="2">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>10</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>43677</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>10</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>43691</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>43748</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="2">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="2">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="2">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A13" s="2">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="2">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="2">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="2">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="2">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="2">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>10</v>
       </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="2">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>10</v>
       </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="2">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>10</v>
       </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="2">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>10</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A22" s="2">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>10</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A23" s="2">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="2">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="2">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A26" s="2">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A27" s="2">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A28" s="2">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A29" s="2">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A30" s="2">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" ht="12.75">
-      <c r="A31" s="2">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="12.75">
+      <c r="A31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2">
         <v>10</v>
       </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="12.75">
-      <c r="A32" s="2">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="12.75">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="12.75">
-      <c r="A33" s="2">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="12.75">
+      <c r="A33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2">
         <v>10</v>
       </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="12.75">
-      <c r="A34" s="2">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="12.75">
+      <c r="A34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2">
         <v>10</v>
       </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="12.75">
-      <c r="A35" s="2">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="12.75">
+      <c r="A35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="12.75">
-      <c r="A36" s="2">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="12.75">
+      <c r="A36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="12.75">
-      <c r="A37" s="2">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="12.75">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="12.75">
-      <c r="A38" s="2">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="12.75">
+      <c r="A38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="12.75">
-      <c r="A39" s="2">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" ht="12.75">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="12.75">
-      <c r="A40" s="2">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="12.75">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" ht="12.75">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="12.75">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>40</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="12.75">
-      <c r="A42" s="2">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" ht="12.75">
+      <c r="A42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" ht="12.75">
-      <c r="A43" s="2">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="12.75">
+      <c r="A43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" ht="12.75">
-      <c r="A44" s="2">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="12.75">
+      <c r="A44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2">
+      <c r="E44" s="2"/>
+      <c r="F44" s="2">
         <v>10</v>
       </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" ht="12.75">
-      <c r="A45" s="2">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="12.75">
+      <c r="A45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" ht="12.75">
-      <c r="A46" s="2">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="12.75">
+      <c r="A46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2">
+      <c r="E46" s="2"/>
+      <c r="F46" s="2">
         <v>10</v>
       </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="12.75">
-      <c r="A47" s="2">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" ht="12.75">
+      <c r="A47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" ht="12.75">
-      <c r="A48" s="2">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" ht="12.75">
+      <c r="A48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" ht="12.75">
-      <c r="A49" s="2">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="12.75">
+      <c r="A49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="2">
+      <c r="E49" s="2"/>
+      <c r="F49" s="2">
         <v>1</v>
       </c>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" ht="12.75"/>
-    <row r="51" spans="1:6" ht="12.75"/>
-    <row r="52" spans="1:6" ht="12.75"/>
-    <row r="53" spans="1:6" ht="12.75"/>
-    <row r="54" spans="1:6" ht="12.75"/>
-    <row r="55" spans="1:6" ht="12.75"/>
-    <row r="56" spans="1:6" ht="12.75"/>
-    <row r="57" spans="1:6" ht="12.75"/>
-    <row r="58" spans="1:6" ht="12.75">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" ht="12.75"/>
+    <row r="51" spans="1:7" ht="12.75"/>
+    <row r="52" spans="1:7" ht="12.75"/>
+    <row r="53" spans="1:7" ht="12.75"/>
+    <row r="54" spans="1:7" ht="12.75"/>
+    <row r="55" spans="1:7" ht="12.75"/>
+    <row r="56" spans="1:7" ht="12.75"/>
+    <row r="57" spans="1:7" ht="12.75"/>
+    <row r="58" spans="1:7" ht="12.75">
       <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:6" ht="12.75"/>
-    <row r="60" spans="1:6" ht="12.75"/>
-    <row r="61" spans="1:6" ht="12.75"/>
-    <row r="62" spans="1:6" ht="12.75"/>
-    <row r="63" spans="1:6" ht="12.75"/>
-    <row r="64" spans="1:6" ht="12.75"/>
+      <c r="B58" s="4"/>
+    </row>
+    <row r="59" spans="1:7" ht="12.75"/>
+    <row r="60" spans="1:7" ht="12.75"/>
+    <row r="61" spans="1:7" ht="12.75"/>
+    <row r="62" spans="1:7" ht="12.75"/>
+    <row r="63" spans="1:7" ht="12.75"/>
+    <row r="64" spans="1:7" ht="12.75"/>
     <row r="65" ht="12.75"/>
     <row r="66" ht="12.75"/>
     <row r="67" ht="12.75"/>

</xml_diff>